<commit_message>
successfully spun up 10 instances of update_pricing
</commit_message>
<xml_diff>
--- a/sql/db_details.xlsx
+++ b/sql/db_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lk/projects/tcg/sql/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F5AB52-B22F-A34E-BFEB-664B264D3B5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B764E86-15ED-FD4E-94F4-D44810617DFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4720" yWindow="760" windowWidth="24240" windowHeight="17780" xr2:uid="{7919C9CE-5EE2-9347-B7C4-F1021AE8E47C}"/>
+    <workbookView xWindow="4720" yWindow="760" windowWidth="23700" windowHeight="15000" xr2:uid="{7919C9CE-5EE2-9347-B7C4-F1021AE8E47C}"/>
   </bookViews>
   <sheets>
     <sheet name="card_prices" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>TCG</t>
   </si>
@@ -84,13 +84,16 @@
   </si>
   <si>
     <t>table: card_prices</t>
+  </si>
+  <si>
+    <t>not yet implemented</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -111,6 +114,21 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,10 +151,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,14 +474,14 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -502,11 +522,14 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>